<commit_message>
desagregaciones - reporte listo
</commit_message>
<xml_diff>
--- a/code/uhmm.xlsx
+++ b/code/uhmm.xlsx
@@ -54,10 +54,10 @@
     <t>+/-</t>
   </si>
   <si>
-    <t>L. inf</t>
+    <t>L inf</t>
   </si>
   <si>
-    <t>L. sup</t>
+    <t>L sup</t>
   </si>
   <si>
     <t>Norm.</t>
@@ -2751,7 +2751,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -3767,7 +3767,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -4783,7 +4783,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -5799,7 +5799,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -6815,7 +6815,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -7831,7 +7831,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -8847,7 +8847,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -9863,7 +9863,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -10879,7 +10879,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -11895,7 +11895,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -12893,7 +12893,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -13891,7 +13891,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -14907,7 +14907,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -15923,7 +15923,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -16939,7 +16939,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -17955,7 +17955,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -18971,7 +18971,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -19987,7 +19987,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -21003,7 +21003,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -22019,7 +22019,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -23059,7 +23059,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -23943,7 +23943,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -24827,7 +24827,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -25843,7 +25843,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -26859,7 +26859,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -27875,7 +27875,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -28891,7 +28891,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -29907,7 +29907,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>
@@ -30923,7 +30923,7 @@
     <col min="6" max="6" width="7.0" customWidth="true"/>
     <col min="7" max="7" width="7.0" customWidth="true"/>
     <col min="8" max="8" width="7.0" customWidth="true"/>
-    <col min="9" max="9" width="13.0" customWidth="true"/>
+    <col min="9" max="9" width="14.0" customWidth="true"/>
     <col min="10" max="10" width="3.0" customWidth="true"/>
     <col min="11" max="11" width="15.0" customWidth="true"/>
     <col min="12" max="12" width="7.0" customWidth="true"/>

</xml_diff>